<commit_message>
Add new version of dashbord V01
</commit_message>
<xml_diff>
--- a/DATA__GEN3-V4.xlsx
+++ b/DATA__GEN3-V4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed Chah\Desktop\gen4-V1-deflection-tool\Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://artedrone.sharepoint.com/sites/SharepointArtedrone/Documents/12. Projets partagés externes/1-HEI/Ahmed-WorkSpace/Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C359C1BE-B758-4602-9A4B-7C4DD917E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{C359C1BE-B758-4602-9A4B-7C4DD917E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9A5DE95-53D1-4D6F-8112-718AB3F0A8C6}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="2175" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="19">
   <si>
     <t>Actuation Angle</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t>Microrobot</t>
-  </si>
-  <si>
-    <t>90°</t>
-  </si>
-  <si>
-    <t>45°</t>
   </si>
   <si>
     <t>GEN3-V4</t>
@@ -678,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E338FDE-009B-4A2A-8A7D-E8F87983CA18}">
   <dimension ref="A1:O313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D308" sqref="D308"/>
+    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159:B313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,10 +693,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
@@ -717,33 +711,33 @@
         <v>8</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="13">
+        <v>90</v>
       </c>
       <c r="C2" s="14">
         <v>180</v>
@@ -766,10 +760,10 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <v>90</v>
       </c>
       <c r="C3" s="1">
         <v>180</v>
@@ -792,10 +786,10 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="6">
+        <v>90</v>
       </c>
       <c r="C4" s="1">
         <v>180</v>
@@ -818,10 +812,10 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="6">
+        <v>90</v>
       </c>
       <c r="C5" s="1">
         <v>180</v>
@@ -844,10 +838,10 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>90</v>
       </c>
       <c r="C6" s="1">
         <v>180</v>
@@ -870,10 +864,10 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="6">
+        <v>90</v>
       </c>
       <c r="C7" s="1">
         <v>180</v>
@@ -896,10 +890,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>90</v>
       </c>
       <c r="C8" s="1">
         <v>180</v>
@@ -922,10 +916,10 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <v>90</v>
       </c>
       <c r="C9" s="1">
         <v>180</v>
@@ -948,10 +942,10 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="6">
+        <v>90</v>
       </c>
       <c r="C10" s="1">
         <v>180</v>
@@ -974,10 +968,10 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="6">
+        <v>90</v>
       </c>
       <c r="C11" s="1">
         <v>180</v>
@@ -1000,10 +994,10 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>90</v>
       </c>
       <c r="C12" s="1">
         <v>180</v>
@@ -1026,10 +1020,10 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>90</v>
       </c>
       <c r="C13" s="1">
         <v>180</v>
@@ -1052,10 +1046,10 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B14" s="6">
+        <v>90</v>
       </c>
       <c r="C14" s="1">
         <v>180</v>
@@ -1078,10 +1072,10 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="6">
+        <v>90</v>
       </c>
       <c r="C15" s="1">
         <v>180</v>
@@ -1104,10 +1098,10 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="6">
+        <v>90</v>
       </c>
       <c r="C16" s="1">
         <v>180</v>
@@ -1130,10 +1124,10 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B17" s="6">
+        <v>90</v>
       </c>
       <c r="C17" s="1">
         <v>180</v>
@@ -1156,10 +1150,10 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="6">
+        <v>90</v>
       </c>
       <c r="C18" s="1">
         <v>180</v>
@@ -1182,10 +1176,10 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="6">
+        <v>90</v>
       </c>
       <c r="C19" s="1">
         <v>180</v>
@@ -1208,10 +1202,10 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B20" s="6">
+        <v>90</v>
       </c>
       <c r="C20" s="1">
         <v>180</v>
@@ -1234,10 +1228,10 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="6">
+        <v>90</v>
       </c>
       <c r="C21" s="1">
         <v>180</v>
@@ -1260,10 +1254,10 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B22" s="6">
+        <v>90</v>
       </c>
       <c r="C22" s="1">
         <v>180</v>
@@ -1286,10 +1280,10 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B23" s="6">
+        <v>90</v>
       </c>
       <c r="C23" s="1">
         <v>180</v>
@@ -1312,10 +1306,10 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B24" s="6">
+        <v>90</v>
       </c>
       <c r="C24" s="1">
         <v>180</v>
@@ -1338,10 +1332,10 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B25" s="6">
+        <v>90</v>
       </c>
       <c r="C25" s="1">
         <v>180</v>
@@ -1364,10 +1358,10 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B26" s="6">
+        <v>90</v>
       </c>
       <c r="C26" s="1">
         <v>180</v>
@@ -1390,10 +1384,10 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B27" s="6">
+        <v>90</v>
       </c>
       <c r="C27" s="1">
         <v>180</v>
@@ -1416,10 +1410,10 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B28" s="6">
+        <v>90</v>
       </c>
       <c r="C28" s="1">
         <v>180</v>
@@ -1442,10 +1436,10 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="6">
+        <v>90</v>
       </c>
       <c r="C29" s="1">
         <v>180</v>
@@ -1468,10 +1462,10 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B30" s="6">
+        <v>90</v>
       </c>
       <c r="C30" s="1">
         <v>180</v>
@@ -1494,10 +1488,10 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B31" s="6">
+        <v>90</v>
       </c>
       <c r="C31" s="1">
         <v>180</v>
@@ -1520,10 +1514,10 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B32" s="6">
+        <v>90</v>
       </c>
       <c r="C32" s="1">
         <v>180</v>
@@ -1546,10 +1540,10 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B33" s="6">
+        <v>90</v>
       </c>
       <c r="C33" s="1">
         <v>180</v>
@@ -1572,10 +1566,10 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B34" s="6">
+        <v>90</v>
       </c>
       <c r="C34" s="1">
         <v>180</v>
@@ -1598,10 +1592,10 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B35" s="6">
+        <v>90</v>
       </c>
       <c r="C35" s="1">
         <v>180</v>
@@ -1624,10 +1618,10 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B36" s="6">
+        <v>90</v>
       </c>
       <c r="C36" s="1">
         <v>180</v>
@@ -1650,10 +1644,10 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B37" s="6">
+        <v>90</v>
       </c>
       <c r="C37" s="1">
         <v>180</v>
@@ -1676,10 +1670,10 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B38" s="6">
+        <v>90</v>
       </c>
       <c r="C38" s="1">
         <v>180</v>
@@ -1702,10 +1696,10 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B39" s="6">
+        <v>90</v>
       </c>
       <c r="C39" s="1">
         <v>180</v>
@@ -1728,10 +1722,10 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B40" s="6">
+        <v>90</v>
       </c>
       <c r="C40" s="1">
         <v>180</v>
@@ -1754,10 +1748,10 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B41" s="6">
+        <v>90</v>
       </c>
       <c r="C41" s="1">
         <v>180</v>
@@ -1780,10 +1774,10 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B42" s="6">
+        <v>90</v>
       </c>
       <c r="C42" s="1">
         <v>180</v>
@@ -1806,10 +1800,10 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B43" s="6">
+        <v>90</v>
       </c>
       <c r="C43" s="1">
         <v>180</v>
@@ -1832,10 +1826,10 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B44" s="6">
+        <v>90</v>
       </c>
       <c r="C44" s="1">
         <v>180</v>
@@ -1858,10 +1852,10 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B45" s="6">
+        <v>90</v>
       </c>
       <c r="C45" s="1">
         <v>180</v>
@@ -1884,10 +1878,10 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B46" s="6">
+        <v>90</v>
       </c>
       <c r="C46" s="1">
         <v>180</v>
@@ -1910,10 +1904,10 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B47" s="6">
+        <v>90</v>
       </c>
       <c r="C47" s="1">
         <v>180</v>
@@ -1936,10 +1930,10 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B48" s="6">
+        <v>90</v>
       </c>
       <c r="C48" s="1">
         <v>180</v>
@@ -1962,10 +1956,10 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B49" s="6">
+        <v>90</v>
       </c>
       <c r="C49" s="1">
         <v>180</v>
@@ -1988,10 +1982,10 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B50" s="6">
+        <v>90</v>
       </c>
       <c r="C50" s="1">
         <v>180</v>
@@ -2014,10 +2008,10 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B51" s="6">
+        <v>90</v>
       </c>
       <c r="C51" s="1">
         <v>180</v>
@@ -2040,10 +2034,10 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B52" s="6">
+        <v>90</v>
       </c>
       <c r="C52" s="1">
         <v>180</v>
@@ -2066,10 +2060,10 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B53" s="6">
+        <v>90</v>
       </c>
       <c r="C53" s="1">
         <v>180</v>
@@ -2092,10 +2086,10 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B54" s="6">
+        <v>90</v>
       </c>
       <c r="C54" s="1">
         <v>180</v>
@@ -2118,10 +2112,10 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B55" s="6">
+        <v>90</v>
       </c>
       <c r="C55" s="1">
         <v>180</v>
@@ -2144,10 +2138,10 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B56" s="6">
+        <v>90</v>
       </c>
       <c r="C56" s="1">
         <v>180</v>
@@ -2170,10 +2164,10 @@
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B57" s="6">
+        <v>90</v>
       </c>
       <c r="C57" s="1">
         <v>180</v>
@@ -2196,10 +2190,10 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B58" s="6">
+        <v>90</v>
       </c>
       <c r="C58" s="1">
         <v>180</v>
@@ -2222,10 +2216,10 @@
     </row>
     <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B59" s="6">
+        <v>90</v>
       </c>
       <c r="C59" s="1">
         <v>180</v>
@@ -2248,10 +2242,10 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B60" s="6">
+        <v>90</v>
       </c>
       <c r="C60" s="1">
         <v>180</v>
@@ -2274,10 +2268,10 @@
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B61" s="6">
+        <v>90</v>
       </c>
       <c r="C61" s="1">
         <v>180</v>
@@ -2300,10 +2294,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B62" s="6">
+        <v>90</v>
       </c>
       <c r="C62" s="1">
         <v>180</v>
@@ -2326,10 +2320,10 @@
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B63" s="6">
+        <v>90</v>
       </c>
       <c r="C63" s="1">
         <v>180</v>
@@ -2352,10 +2346,10 @@
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B64" s="6">
+        <v>90</v>
       </c>
       <c r="C64" s="1">
         <v>180</v>
@@ -2378,10 +2372,10 @@
     </row>
     <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B65" s="6">
+        <v>90</v>
       </c>
       <c r="C65" s="1">
         <v>180</v>
@@ -2404,10 +2398,10 @@
     </row>
     <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B66" s="6">
+        <v>90</v>
       </c>
       <c r="C66" s="1">
         <v>180</v>
@@ -2430,10 +2424,10 @@
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B67" s="6">
+        <v>90</v>
       </c>
       <c r="C67" s="1">
         <v>180</v>
@@ -2456,10 +2450,10 @@
     </row>
     <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B68" s="6">
+        <v>90</v>
       </c>
       <c r="C68" s="1">
         <v>180</v>
@@ -2482,10 +2476,10 @@
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B69" s="6">
+        <v>90</v>
       </c>
       <c r="C69" s="1">
         <v>180</v>
@@ -2508,10 +2502,10 @@
     </row>
     <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B70" s="6">
+        <v>90</v>
       </c>
       <c r="C70" s="1">
         <v>180</v>
@@ -2534,10 +2528,10 @@
     </row>
     <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B71" s="6">
+        <v>90</v>
       </c>
       <c r="C71" s="1">
         <v>180</v>
@@ -2560,10 +2554,10 @@
     </row>
     <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>13</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B72" s="6">
+        <v>90</v>
       </c>
       <c r="C72" s="1">
         <v>180</v>
@@ -2586,10 +2580,10 @@
     </row>
     <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B73" s="6">
+        <v>90</v>
       </c>
       <c r="C73" s="1">
         <v>180</v>
@@ -2612,10 +2606,10 @@
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B74" s="6">
+        <v>90</v>
       </c>
       <c r="C74" s="1">
         <v>180</v>
@@ -2638,10 +2632,10 @@
     </row>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>13</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B75" s="6">
+        <v>90</v>
       </c>
       <c r="C75" s="1">
         <v>180</v>
@@ -2664,10 +2658,10 @@
     </row>
     <row r="76" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B76" s="6">
+        <v>90</v>
       </c>
       <c r="C76" s="1">
         <v>180</v>
@@ -2690,10 +2684,10 @@
     </row>
     <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>13</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B77" s="6">
+        <v>90</v>
       </c>
       <c r="C77" s="1">
         <v>180</v>
@@ -2716,10 +2710,10 @@
     </row>
     <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B78" s="6">
+        <v>90</v>
       </c>
       <c r="C78" s="1">
         <v>180</v>
@@ -2742,10 +2736,10 @@
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>13</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B79" s="6">
+        <v>90</v>
       </c>
       <c r="C79" s="1">
         <v>180</v>
@@ -2768,10 +2762,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B80" s="6">
+        <v>90</v>
       </c>
       <c r="C80" s="1">
         <v>0</v>
@@ -2794,10 +2788,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B81" s="6">
+        <v>90</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
@@ -2820,10 +2814,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>13</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B82" s="6">
+        <v>90</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
@@ -2846,10 +2840,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B83" s="6">
+        <v>90</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
@@ -2872,10 +2866,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>13</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B84" s="6">
+        <v>90</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
@@ -2898,10 +2892,10 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B85" s="6">
+        <v>90</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
@@ -2924,10 +2918,10 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>13</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B86" s="6">
+        <v>90</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
@@ -2950,10 +2944,10 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B87" s="6">
+        <v>90</v>
       </c>
       <c r="C87" s="1">
         <v>0</v>
@@ -2976,10 +2970,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>13</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B88" s="6">
+        <v>90</v>
       </c>
       <c r="C88" s="1">
         <v>0</v>
@@ -3002,10 +2996,10 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>13</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B89" s="6">
+        <v>90</v>
       </c>
       <c r="C89" s="1">
         <v>0</v>
@@ -3028,10 +3022,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>13</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B90" s="6">
+        <v>90</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
@@ -3054,10 +3048,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>13</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B91" s="6">
+        <v>90</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
@@ -3080,10 +3074,10 @@
     </row>
     <row r="92" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>13</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B92" s="6">
+        <v>90</v>
       </c>
       <c r="C92" s="1">
         <v>0</v>
@@ -3106,10 +3100,10 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>13</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B93" s="6">
+        <v>90</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -3132,10 +3126,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>13</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B94" s="6">
+        <v>90</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
@@ -3158,10 +3152,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>13</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B95" s="6">
+        <v>90</v>
       </c>
       <c r="C95" s="1">
         <v>0</v>
@@ -3184,10 +3178,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>13</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B96" s="6">
+        <v>90</v>
       </c>
       <c r="C96" s="1">
         <v>0</v>
@@ -3210,10 +3204,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>13</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B97" s="6">
+        <v>90</v>
       </c>
       <c r="C97" s="1">
         <v>0</v>
@@ -3236,10 +3230,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>13</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B98" s="6">
+        <v>90</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
@@ -3262,10 +3256,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>13</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B99" s="6">
+        <v>90</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
@@ -3288,10 +3282,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>13</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B100" s="6">
+        <v>90</v>
       </c>
       <c r="C100" s="1">
         <v>0</v>
@@ -3314,10 +3308,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B101" s="6">
+        <v>90</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
@@ -3340,10 +3334,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B102" s="6">
+        <v>90</v>
       </c>
       <c r="C102" s="1">
         <v>0</v>
@@ -3366,10 +3360,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>13</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B103" s="6">
+        <v>90</v>
       </c>
       <c r="C103" s="1">
         <v>0</v>
@@ -3392,10 +3386,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>13</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B104" s="6">
+        <v>90</v>
       </c>
       <c r="C104" s="1">
         <v>0</v>
@@ -3418,10 +3412,10 @@
     </row>
     <row r="105" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>13</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B105" s="6">
+        <v>90</v>
       </c>
       <c r="C105" s="1">
         <v>0</v>
@@ -3444,10 +3438,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>13</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B106" s="6">
+        <v>90</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
@@ -3470,10 +3464,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>13</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B107" s="6">
+        <v>90</v>
       </c>
       <c r="C107" s="1">
         <v>0</v>
@@ -3496,10 +3490,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>13</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B108" s="6">
+        <v>90</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
@@ -3522,10 +3516,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B109" s="6">
+        <v>90</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
@@ -3548,10 +3542,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>13</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B110" s="6">
+        <v>90</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
@@ -3574,10 +3568,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B111" s="6">
+        <v>90</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
@@ -3600,10 +3594,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>13</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B112" s="6">
+        <v>90</v>
       </c>
       <c r="C112" s="1">
         <v>0</v>
@@ -3626,10 +3620,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>13</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B113" s="6">
+        <v>90</v>
       </c>
       <c r="C113" s="1">
         <v>0</v>
@@ -3652,10 +3646,10 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B114" s="6">
+        <v>90</v>
       </c>
       <c r="C114" s="1">
         <v>0</v>
@@ -3678,10 +3672,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>13</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B115" s="6">
+        <v>90</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
@@ -3704,10 +3698,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>13</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B116" s="6">
+        <v>90</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
@@ -3730,10 +3724,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>13</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B117" s="6">
+        <v>90</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -3756,10 +3750,10 @@
     </row>
     <row r="118" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>13</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B118" s="6">
+        <v>90</v>
       </c>
       <c r="C118" s="1">
         <v>0</v>
@@ -3782,10 +3776,10 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B119" s="6">
+        <v>90</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
@@ -3808,10 +3802,10 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>13</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B120" s="6">
+        <v>90</v>
       </c>
       <c r="C120" s="1">
         <v>0</v>
@@ -3834,10 +3828,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>13</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B121" s="6">
+        <v>90</v>
       </c>
       <c r="C121" s="1">
         <v>0</v>
@@ -3860,10 +3854,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>13</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B122" s="6">
+        <v>90</v>
       </c>
       <c r="C122" s="1">
         <v>0</v>
@@ -3886,10 +3880,10 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>13</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B123" s="6">
+        <v>90</v>
       </c>
       <c r="C123" s="1">
         <v>0</v>
@@ -3912,10 +3906,10 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>13</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B124" s="6">
+        <v>90</v>
       </c>
       <c r="C124" s="1">
         <v>0</v>
@@ -3938,10 +3932,10 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>13</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B125" s="6">
+        <v>90</v>
       </c>
       <c r="C125" s="1">
         <v>0</v>
@@ -3964,10 +3958,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>13</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B126" s="6">
+        <v>90</v>
       </c>
       <c r="C126" s="1">
         <v>0</v>
@@ -3990,10 +3984,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>13</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B127" s="6">
+        <v>90</v>
       </c>
       <c r="C127" s="1">
         <v>0</v>
@@ -4016,10 +4010,10 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>13</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B128" s="6">
+        <v>90</v>
       </c>
       <c r="C128" s="1">
         <v>0</v>
@@ -4042,10 +4036,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>13</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B129" s="6">
+        <v>90</v>
       </c>
       <c r="C129" s="1">
         <v>0</v>
@@ -4068,10 +4062,10 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>13</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B130" s="6">
+        <v>90</v>
       </c>
       <c r="C130" s="1">
         <v>0</v>
@@ -4094,10 +4088,10 @@
     </row>
     <row r="131" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>13</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B131" s="6">
+        <v>90</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
@@ -4120,10 +4114,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>13</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B132" s="6">
+        <v>90</v>
       </c>
       <c r="C132" s="1">
         <v>0</v>
@@ -4146,10 +4140,10 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>13</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B133" s="6">
+        <v>90</v>
       </c>
       <c r="C133" s="1">
         <v>0</v>
@@ -4172,10 +4166,10 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>13</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B134" s="6">
+        <v>90</v>
       </c>
       <c r="C134" s="1">
         <v>0</v>
@@ -4198,10 +4192,10 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>13</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B135" s="6">
+        <v>90</v>
       </c>
       <c r="C135" s="1">
         <v>0</v>
@@ -4224,10 +4218,10 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>13</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B136" s="6">
+        <v>90</v>
       </c>
       <c r="C136" s="1">
         <v>0</v>
@@ -4250,10 +4244,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>13</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B137" s="6">
+        <v>90</v>
       </c>
       <c r="C137" s="1">
         <v>0</v>
@@ -4276,10 +4270,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>13</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B138" s="6">
+        <v>90</v>
       </c>
       <c r="C138" s="1">
         <v>0</v>
@@ -4302,10 +4296,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>13</v>
-      </c>
-      <c r="B139" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B139" s="6">
+        <v>90</v>
       </c>
       <c r="C139" s="1">
         <v>0</v>
@@ -4328,10 +4322,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>13</v>
-      </c>
-      <c r="B140" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B140" s="6">
+        <v>90</v>
       </c>
       <c r="C140" s="1">
         <v>0</v>
@@ -4354,10 +4348,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>13</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B141" s="6">
+        <v>90</v>
       </c>
       <c r="C141" s="1">
         <v>0</v>
@@ -4380,10 +4374,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>13</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B142" s="6">
+        <v>90</v>
       </c>
       <c r="C142" s="1">
         <v>0</v>
@@ -4406,10 +4400,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>13</v>
-      </c>
-      <c r="B143" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B143" s="6">
+        <v>90</v>
       </c>
       <c r="C143" s="1">
         <v>0</v>
@@ -4432,10 +4426,10 @@
     </row>
     <row r="144" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>13</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B144" s="6">
+        <v>90</v>
       </c>
       <c r="C144" s="1">
         <v>0</v>
@@ -4458,10 +4452,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>13</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B145" s="6">
+        <v>90</v>
       </c>
       <c r="C145" s="1">
         <v>0</v>
@@ -4484,10 +4478,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>13</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B146" s="6">
+        <v>90</v>
       </c>
       <c r="C146" s="1">
         <v>0</v>
@@ -4510,10 +4504,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>13</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B147" s="6">
+        <v>90</v>
       </c>
       <c r="C147" s="1">
         <v>0</v>
@@ -4536,10 +4530,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>13</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B148" s="6">
+        <v>90</v>
       </c>
       <c r="C148" s="1">
         <v>0</v>
@@ -4562,10 +4556,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>13</v>
-      </c>
-      <c r="B149" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B149" s="6">
+        <v>90</v>
       </c>
       <c r="C149" s="1">
         <v>0</v>
@@ -4588,10 +4582,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>13</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B150" s="6">
+        <v>90</v>
       </c>
       <c r="C150" s="1">
         <v>0</v>
@@ -4614,10 +4608,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>13</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B151" s="6">
+        <v>90</v>
       </c>
       <c r="C151" s="1">
         <v>0</v>
@@ -4640,10 +4634,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>13</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B152" s="6">
+        <v>90</v>
       </c>
       <c r="C152" s="1">
         <v>0</v>
@@ -4666,10 +4660,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>13</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B153" s="6">
+        <v>90</v>
       </c>
       <c r="C153" s="1">
         <v>0</v>
@@ -4692,10 +4686,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>13</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B154" s="6">
+        <v>90</v>
       </c>
       <c r="C154" s="1">
         <v>0</v>
@@ -4718,10 +4712,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>13</v>
-      </c>
-      <c r="B155" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B155" s="6">
+        <v>90</v>
       </c>
       <c r="C155" s="1">
         <v>0</v>
@@ -4744,10 +4738,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>13</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B156" s="6">
+        <v>90</v>
       </c>
       <c r="C156" s="1">
         <v>0</v>
@@ -4770,10 +4764,10 @@
     </row>
     <row r="157" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>13</v>
-      </c>
-      <c r="B157" s="6" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="B157" s="6">
+        <v>90</v>
       </c>
       <c r="C157" s="1">
         <v>0</v>
@@ -4796,10 +4790,10 @@
     </row>
     <row r="158" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>13</v>
-      </c>
-      <c r="B158" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B158" s="13">
+        <v>45</v>
       </c>
       <c r="C158" s="1">
         <v>180</v>
@@ -4822,10 +4816,10 @@
     </row>
     <row r="159" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>13</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B159" s="6">
+        <v>45</v>
       </c>
       <c r="C159" s="1">
         <v>180</v>
@@ -4848,10 +4842,10 @@
     </row>
     <row r="160" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>13</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B160" s="6">
+        <v>45</v>
       </c>
       <c r="C160" s="1">
         <v>180</v>
@@ -4874,10 +4868,10 @@
     </row>
     <row r="161" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>13</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B161" s="6">
+        <v>45</v>
       </c>
       <c r="C161" s="1">
         <v>180</v>
@@ -4900,10 +4894,10 @@
     </row>
     <row r="162" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>13</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B162" s="6">
+        <v>45</v>
       </c>
       <c r="C162" s="1">
         <v>180</v>
@@ -4926,10 +4920,10 @@
     </row>
     <row r="163" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>13</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B163" s="6">
+        <v>45</v>
       </c>
       <c r="C163" s="1">
         <v>180</v>
@@ -4952,10 +4946,10 @@
     </row>
     <row r="164" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>13</v>
-      </c>
-      <c r="B164" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B164" s="6">
+        <v>45</v>
       </c>
       <c r="C164" s="1">
         <v>180</v>
@@ -4978,10 +4972,10 @@
     </row>
     <row r="165" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>13</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B165" s="6">
+        <v>45</v>
       </c>
       <c r="C165" s="1">
         <v>180</v>
@@ -5004,10 +4998,10 @@
     </row>
     <row r="166" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>13</v>
-      </c>
-      <c r="B166" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B166" s="6">
+        <v>45</v>
       </c>
       <c r="C166" s="1">
         <v>180</v>
@@ -5030,10 +5024,10 @@
     </row>
     <row r="167" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>13</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B167" s="6">
+        <v>45</v>
       </c>
       <c r="C167" s="1">
         <v>180</v>
@@ -5056,10 +5050,10 @@
     </row>
     <row r="168" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>13</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B168" s="6">
+        <v>45</v>
       </c>
       <c r="C168" s="1">
         <v>180</v>
@@ -5082,10 +5076,10 @@
     </row>
     <row r="169" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>13</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B169" s="6">
+        <v>45</v>
       </c>
       <c r="C169" s="1">
         <v>180</v>
@@ -5108,10 +5102,10 @@
     </row>
     <row r="170" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>13</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B170" s="6">
+        <v>45</v>
       </c>
       <c r="C170" s="1">
         <v>180</v>
@@ -5134,10 +5128,10 @@
     </row>
     <row r="171" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>13</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B171" s="6">
+        <v>45</v>
       </c>
       <c r="C171" s="1">
         <v>180</v>
@@ -5160,10 +5154,10 @@
     </row>
     <row r="172" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>13</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B172" s="6">
+        <v>45</v>
       </c>
       <c r="C172" s="1">
         <v>180</v>
@@ -5186,10 +5180,10 @@
     </row>
     <row r="173" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>13</v>
-      </c>
-      <c r="B173" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B173" s="6">
+        <v>45</v>
       </c>
       <c r="C173" s="1">
         <v>180</v>
@@ -5212,10 +5206,10 @@
     </row>
     <row r="174" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>13</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B174" s="6">
+        <v>45</v>
       </c>
       <c r="C174" s="1">
         <v>180</v>
@@ -5238,10 +5232,10 @@
     </row>
     <row r="175" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>13</v>
-      </c>
-      <c r="B175" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B175" s="6">
+        <v>45</v>
       </c>
       <c r="C175" s="1">
         <v>180</v>
@@ -5264,10 +5258,10 @@
     </row>
     <row r="176" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>13</v>
-      </c>
-      <c r="B176" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B176" s="6">
+        <v>45</v>
       </c>
       <c r="C176" s="1">
         <v>180</v>
@@ -5290,10 +5284,10 @@
     </row>
     <row r="177" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>13</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B177" s="6">
+        <v>45</v>
       </c>
       <c r="C177" s="1">
         <v>180</v>
@@ -5316,10 +5310,10 @@
     </row>
     <row r="178" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>13</v>
-      </c>
-      <c r="B178" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B178" s="6">
+        <v>45</v>
       </c>
       <c r="C178" s="1">
         <v>180</v>
@@ -5342,10 +5336,10 @@
     </row>
     <row r="179" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>13</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B179" s="6">
+        <v>45</v>
       </c>
       <c r="C179" s="1">
         <v>180</v>
@@ -5368,10 +5362,10 @@
     </row>
     <row r="180" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>13</v>
-      </c>
-      <c r="B180" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B180" s="6">
+        <v>45</v>
       </c>
       <c r="C180" s="1">
         <v>180</v>
@@ -5394,10 +5388,10 @@
     </row>
     <row r="181" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>13</v>
-      </c>
-      <c r="B181" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B181" s="6">
+        <v>45</v>
       </c>
       <c r="C181" s="1">
         <v>180</v>
@@ -5420,10 +5414,10 @@
     </row>
     <row r="182" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>13</v>
-      </c>
-      <c r="B182" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B182" s="6">
+        <v>45</v>
       </c>
       <c r="C182" s="1">
         <v>180</v>
@@ -5446,10 +5440,10 @@
     </row>
     <row r="183" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>13</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B183" s="6">
+        <v>45</v>
       </c>
       <c r="C183" s="1">
         <v>180</v>
@@ -5472,10 +5466,10 @@
     </row>
     <row r="184" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>13</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B184" s="6">
+        <v>45</v>
       </c>
       <c r="C184" s="1">
         <v>180</v>
@@ -5498,10 +5492,10 @@
     </row>
     <row r="185" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>13</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B185" s="6">
+        <v>45</v>
       </c>
       <c r="C185" s="1">
         <v>180</v>
@@ -5524,10 +5518,10 @@
     </row>
     <row r="186" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>13</v>
-      </c>
-      <c r="B186" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B186" s="6">
+        <v>45</v>
       </c>
       <c r="C186" s="1">
         <v>180</v>
@@ -5550,10 +5544,10 @@
     </row>
     <row r="187" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>13</v>
-      </c>
-      <c r="B187" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B187" s="6">
+        <v>45</v>
       </c>
       <c r="C187" s="1">
         <v>180</v>
@@ -5576,10 +5570,10 @@
     </row>
     <row r="188" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>13</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B188" s="6">
+        <v>45</v>
       </c>
       <c r="C188" s="1">
         <v>180</v>
@@ -5602,10 +5596,10 @@
     </row>
     <row r="189" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>13</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B189" s="6">
+        <v>45</v>
       </c>
       <c r="C189" s="1">
         <v>180</v>
@@ -5628,10 +5622,10 @@
     </row>
     <row r="190" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>13</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B190" s="6">
+        <v>45</v>
       </c>
       <c r="C190" s="1">
         <v>180</v>
@@ -5654,10 +5648,10 @@
     </row>
     <row r="191" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>13</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B191" s="6">
+        <v>45</v>
       </c>
       <c r="C191" s="1">
         <v>180</v>
@@ -5680,10 +5674,10 @@
     </row>
     <row r="192" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>13</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B192" s="6">
+        <v>45</v>
       </c>
       <c r="C192" s="1">
         <v>180</v>
@@ -5706,10 +5700,10 @@
     </row>
     <row r="193" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>13</v>
-      </c>
-      <c r="B193" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B193" s="6">
+        <v>45</v>
       </c>
       <c r="C193" s="1">
         <v>180</v>
@@ -5732,10 +5726,10 @@
     </row>
     <row r="194" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>13</v>
-      </c>
-      <c r="B194" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B194" s="6">
+        <v>45</v>
       </c>
       <c r="C194" s="1">
         <v>180</v>
@@ -5758,10 +5752,10 @@
     </row>
     <row r="195" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>13</v>
-      </c>
-      <c r="B195" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B195" s="6">
+        <v>45</v>
       </c>
       <c r="C195" s="1">
         <v>180</v>
@@ -5784,10 +5778,10 @@
     </row>
     <row r="196" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>13</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B196" s="6">
+        <v>45</v>
       </c>
       <c r="C196" s="1">
         <v>180</v>
@@ -5810,10 +5804,10 @@
     </row>
     <row r="197" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>13</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B197" s="6">
+        <v>45</v>
       </c>
       <c r="C197" s="1">
         <v>180</v>
@@ -5836,10 +5830,10 @@
     </row>
     <row r="198" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>13</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B198" s="6">
+        <v>45</v>
       </c>
       <c r="C198" s="1">
         <v>180</v>
@@ -5862,10 +5856,10 @@
     </row>
     <row r="199" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>13</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B199" s="6">
+        <v>45</v>
       </c>
       <c r="C199" s="1">
         <v>180</v>
@@ -5888,10 +5882,10 @@
     </row>
     <row r="200" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>13</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B200" s="6">
+        <v>45</v>
       </c>
       <c r="C200" s="1">
         <v>180</v>
@@ -5914,10 +5908,10 @@
     </row>
     <row r="201" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>13</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B201" s="6">
+        <v>45</v>
       </c>
       <c r="C201" s="1">
         <v>180</v>
@@ -5940,10 +5934,10 @@
     </row>
     <row r="202" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>13</v>
-      </c>
-      <c r="B202" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B202" s="6">
+        <v>45</v>
       </c>
       <c r="C202" s="1">
         <v>180</v>
@@ -5966,10 +5960,10 @@
     </row>
     <row r="203" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>13</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B203" s="6">
+        <v>45</v>
       </c>
       <c r="C203" s="1">
         <v>180</v>
@@ -5992,10 +5986,10 @@
     </row>
     <row r="204" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>13</v>
-      </c>
-      <c r="B204" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B204" s="6">
+        <v>45</v>
       </c>
       <c r="C204" s="1">
         <v>180</v>
@@ -6018,10 +6012,10 @@
     </row>
     <row r="205" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>13</v>
-      </c>
-      <c r="B205" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B205" s="6">
+        <v>45</v>
       </c>
       <c r="C205" s="1">
         <v>180</v>
@@ -6044,10 +6038,10 @@
     </row>
     <row r="206" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>13</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B206" s="6">
+        <v>45</v>
       </c>
       <c r="C206" s="1">
         <v>180</v>
@@ -6070,10 +6064,10 @@
     </row>
     <row r="207" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>13</v>
-      </c>
-      <c r="B207" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B207" s="6">
+        <v>45</v>
       </c>
       <c r="C207" s="1">
         <v>180</v>
@@ -6096,10 +6090,10 @@
     </row>
     <row r="208" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>13</v>
-      </c>
-      <c r="B208" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B208" s="6">
+        <v>45</v>
       </c>
       <c r="C208" s="1">
         <v>180</v>
@@ -6122,10 +6116,10 @@
     </row>
     <row r="209" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>13</v>
-      </c>
-      <c r="B209" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B209" s="6">
+        <v>45</v>
       </c>
       <c r="C209" s="1">
         <v>180</v>
@@ -6148,10 +6142,10 @@
     </row>
     <row r="210" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>13</v>
-      </c>
-      <c r="B210" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B210" s="6">
+        <v>45</v>
       </c>
       <c r="C210" s="1">
         <v>180</v>
@@ -6174,10 +6168,10 @@
     </row>
     <row r="211" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>13</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B211" s="6">
+        <v>45</v>
       </c>
       <c r="C211" s="1">
         <v>180</v>
@@ -6200,10 +6194,10 @@
     </row>
     <row r="212" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>13</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B212" s="6">
+        <v>45</v>
       </c>
       <c r="C212" s="1">
         <v>180</v>
@@ -6226,10 +6220,10 @@
     </row>
     <row r="213" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>13</v>
-      </c>
-      <c r="B213" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B213" s="6">
+        <v>45</v>
       </c>
       <c r="C213" s="1">
         <v>180</v>
@@ -6252,10 +6246,10 @@
     </row>
     <row r="214" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>13</v>
-      </c>
-      <c r="B214" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B214" s="6">
+        <v>45</v>
       </c>
       <c r="C214" s="1">
         <v>180</v>
@@ -6278,10 +6272,10 @@
     </row>
     <row r="215" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>13</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B215" s="6">
+        <v>45</v>
       </c>
       <c r="C215" s="1">
         <v>180</v>
@@ -6304,10 +6298,10 @@
     </row>
     <row r="216" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>13</v>
-      </c>
-      <c r="B216" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B216" s="6">
+        <v>45</v>
       </c>
       <c r="C216" s="1">
         <v>180</v>
@@ -6330,10 +6324,10 @@
     </row>
     <row r="217" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>13</v>
-      </c>
-      <c r="B217" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B217" s="6">
+        <v>45</v>
       </c>
       <c r="C217" s="1">
         <v>180</v>
@@ -6356,10 +6350,10 @@
     </row>
     <row r="218" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>13</v>
-      </c>
-      <c r="B218" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B218" s="6">
+        <v>45</v>
       </c>
       <c r="C218" s="1">
         <v>180</v>
@@ -6382,10 +6376,10 @@
     </row>
     <row r="219" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>13</v>
-      </c>
-      <c r="B219" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B219" s="6">
+        <v>45</v>
       </c>
       <c r="C219" s="1">
         <v>180</v>
@@ -6408,10 +6402,10 @@
     </row>
     <row r="220" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>13</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B220" s="6">
+        <v>45</v>
       </c>
       <c r="C220" s="1">
         <v>180</v>
@@ -6434,10 +6428,10 @@
     </row>
     <row r="221" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>13</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B221" s="6">
+        <v>45</v>
       </c>
       <c r="C221" s="1">
         <v>180</v>
@@ -6460,10 +6454,10 @@
     </row>
     <row r="222" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>13</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B222" s="6">
+        <v>45</v>
       </c>
       <c r="C222" s="1">
         <v>180</v>
@@ -6486,10 +6480,10 @@
     </row>
     <row r="223" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>13</v>
-      </c>
-      <c r="B223" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B223" s="6">
+        <v>45</v>
       </c>
       <c r="C223" s="1">
         <v>180</v>
@@ -6512,10 +6506,10 @@
     </row>
     <row r="224" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>13</v>
-      </c>
-      <c r="B224" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B224" s="6">
+        <v>45</v>
       </c>
       <c r="C224" s="1">
         <v>180</v>
@@ -6538,10 +6532,10 @@
     </row>
     <row r="225" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>13</v>
-      </c>
-      <c r="B225" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B225" s="6">
+        <v>45</v>
       </c>
       <c r="C225" s="1">
         <v>180</v>
@@ -6564,10 +6558,10 @@
     </row>
     <row r="226" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>13</v>
-      </c>
-      <c r="B226" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B226" s="6">
+        <v>45</v>
       </c>
       <c r="C226" s="1">
         <v>180</v>
@@ -6590,10 +6584,10 @@
     </row>
     <row r="227" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>13</v>
-      </c>
-      <c r="B227" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B227" s="6">
+        <v>45</v>
       </c>
       <c r="C227" s="1">
         <v>180</v>
@@ -6616,10 +6610,10 @@
     </row>
     <row r="228" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>13</v>
-      </c>
-      <c r="B228" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B228" s="6">
+        <v>45</v>
       </c>
       <c r="C228" s="1">
         <v>180</v>
@@ -6642,10 +6636,10 @@
     </row>
     <row r="229" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>13</v>
-      </c>
-      <c r="B229" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B229" s="6">
+        <v>45</v>
       </c>
       <c r="C229" s="1">
         <v>180</v>
@@ -6668,10 +6662,10 @@
     </row>
     <row r="230" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>13</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B230" s="6">
+        <v>45</v>
       </c>
       <c r="C230" s="1">
         <v>180</v>
@@ -6694,10 +6688,10 @@
     </row>
     <row r="231" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>13</v>
-      </c>
-      <c r="B231" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B231" s="6">
+        <v>45</v>
       </c>
       <c r="C231" s="1">
         <v>180</v>
@@ -6720,10 +6714,10 @@
     </row>
     <row r="232" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>13</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B232" s="6">
+        <v>45</v>
       </c>
       <c r="C232" s="1">
         <v>180</v>
@@ -6746,10 +6740,10 @@
     </row>
     <row r="233" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>13</v>
-      </c>
-      <c r="B233" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B233" s="6">
+        <v>45</v>
       </c>
       <c r="C233" s="1">
         <v>180</v>
@@ -6772,10 +6766,10 @@
     </row>
     <row r="234" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>13</v>
-      </c>
-      <c r="B234" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B234" s="6">
+        <v>45</v>
       </c>
       <c r="C234" s="1">
         <v>180</v>
@@ -6798,10 +6792,10 @@
     </row>
     <row r="235" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>13</v>
-      </c>
-      <c r="B235" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B235" s="6">
+        <v>45</v>
       </c>
       <c r="C235" s="1">
         <v>180</v>
@@ -6824,10 +6818,10 @@
     </row>
     <row r="236" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>13</v>
-      </c>
-      <c r="B236" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B236" s="6">
+        <v>45</v>
       </c>
       <c r="C236" s="1">
         <v>0</v>
@@ -6850,10 +6844,10 @@
     </row>
     <row r="237" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B237" s="6">
+        <v>45</v>
       </c>
       <c r="C237" s="1">
         <v>0</v>
@@ -6876,10 +6870,10 @@
     </row>
     <row r="238" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>13</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B238" s="6">
+        <v>45</v>
       </c>
       <c r="C238" s="1">
         <v>0</v>
@@ -6902,10 +6896,10 @@
     </row>
     <row r="239" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>13</v>
-      </c>
-      <c r="B239" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B239" s="6">
+        <v>45</v>
       </c>
       <c r="C239" s="1">
         <v>0</v>
@@ -6928,10 +6922,10 @@
     </row>
     <row r="240" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>13</v>
-      </c>
-      <c r="B240" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B240" s="6">
+        <v>45</v>
       </c>
       <c r="C240" s="1">
         <v>0</v>
@@ -6954,10 +6948,10 @@
     </row>
     <row r="241" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>13</v>
-      </c>
-      <c r="B241" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B241" s="6">
+        <v>45</v>
       </c>
       <c r="C241" s="1">
         <v>0</v>
@@ -6980,10 +6974,10 @@
     </row>
     <row r="242" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B242" s="6">
+        <v>45</v>
       </c>
       <c r="C242" s="1">
         <v>0</v>
@@ -7006,10 +7000,10 @@
     </row>
     <row r="243" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>13</v>
-      </c>
-      <c r="B243" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B243" s="6">
+        <v>45</v>
       </c>
       <c r="C243" s="1">
         <v>0</v>
@@ -7032,10 +7026,10 @@
     </row>
     <row r="244" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>13</v>
-      </c>
-      <c r="B244" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B244" s="6">
+        <v>45</v>
       </c>
       <c r="C244" s="1">
         <v>0</v>
@@ -7058,10 +7052,10 @@
     </row>
     <row r="245" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>13</v>
-      </c>
-      <c r="B245" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B245" s="6">
+        <v>45</v>
       </c>
       <c r="C245" s="1">
         <v>0</v>
@@ -7084,10 +7078,10 @@
     </row>
     <row r="246" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>13</v>
-      </c>
-      <c r="B246" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B246" s="6">
+        <v>45</v>
       </c>
       <c r="C246" s="1">
         <v>0</v>
@@ -7110,10 +7104,10 @@
     </row>
     <row r="247" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>13</v>
-      </c>
-      <c r="B247" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B247" s="6">
+        <v>45</v>
       </c>
       <c r="C247" s="1">
         <v>0</v>
@@ -7136,10 +7130,10 @@
     </row>
     <row r="248" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>13</v>
-      </c>
-      <c r="B248" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B248" s="6">
+        <v>45</v>
       </c>
       <c r="C248" s="1">
         <v>0</v>
@@ -7162,10 +7156,10 @@
     </row>
     <row r="249" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>13</v>
-      </c>
-      <c r="B249" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B249" s="6">
+        <v>45</v>
       </c>
       <c r="C249" s="1">
         <v>0</v>
@@ -7188,10 +7182,10 @@
     </row>
     <row r="250" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>13</v>
-      </c>
-      <c r="B250" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B250" s="6">
+        <v>45</v>
       </c>
       <c r="C250" s="1">
         <v>0</v>
@@ -7214,10 +7208,10 @@
     </row>
     <row r="251" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>13</v>
-      </c>
-      <c r="B251" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B251" s="6">
+        <v>45</v>
       </c>
       <c r="C251" s="1">
         <v>0</v>
@@ -7240,10 +7234,10 @@
     </row>
     <row r="252" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>13</v>
-      </c>
-      <c r="B252" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B252" s="6">
+        <v>45</v>
       </c>
       <c r="C252" s="1">
         <v>0</v>
@@ -7266,10 +7260,10 @@
     </row>
     <row r="253" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>13</v>
-      </c>
-      <c r="B253" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B253" s="6">
+        <v>45</v>
       </c>
       <c r="C253" s="1">
         <v>0</v>
@@ -7292,10 +7286,10 @@
     </row>
     <row r="254" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>13</v>
-      </c>
-      <c r="B254" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B254" s="6">
+        <v>45</v>
       </c>
       <c r="C254" s="1">
         <v>0</v>
@@ -7318,10 +7312,10 @@
     </row>
     <row r="255" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>13</v>
-      </c>
-      <c r="B255" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B255" s="6">
+        <v>45</v>
       </c>
       <c r="C255" s="1">
         <v>0</v>
@@ -7344,10 +7338,10 @@
     </row>
     <row r="256" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>13</v>
-      </c>
-      <c r="B256" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B256" s="6">
+        <v>45</v>
       </c>
       <c r="C256" s="1">
         <v>0</v>
@@ -7370,10 +7364,10 @@
     </row>
     <row r="257" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>13</v>
-      </c>
-      <c r="B257" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B257" s="6">
+        <v>45</v>
       </c>
       <c r="C257" s="1">
         <v>0</v>
@@ -7396,10 +7390,10 @@
     </row>
     <row r="258" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>13</v>
-      </c>
-      <c r="B258" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B258" s="6">
+        <v>45</v>
       </c>
       <c r="C258" s="1">
         <v>0</v>
@@ -7422,10 +7416,10 @@
     </row>
     <row r="259" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>13</v>
-      </c>
-      <c r="B259" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B259" s="6">
+        <v>45</v>
       </c>
       <c r="C259" s="1">
         <v>0</v>
@@ -7448,10 +7442,10 @@
     </row>
     <row r="260" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>13</v>
-      </c>
-      <c r="B260" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B260" s="6">
+        <v>45</v>
       </c>
       <c r="C260" s="1">
         <v>0</v>
@@ -7474,10 +7468,10 @@
     </row>
     <row r="261" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>13</v>
-      </c>
-      <c r="B261" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B261" s="6">
+        <v>45</v>
       </c>
       <c r="C261" s="1">
         <v>0</v>
@@ -7500,10 +7494,10 @@
     </row>
     <row r="262" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>13</v>
-      </c>
-      <c r="B262" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B262" s="6">
+        <v>45</v>
       </c>
       <c r="C262" s="1">
         <v>0</v>
@@ -7526,10 +7520,10 @@
     </row>
     <row r="263" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>13</v>
-      </c>
-      <c r="B263" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B263" s="6">
+        <v>45</v>
       </c>
       <c r="C263" s="1">
         <v>0</v>
@@ -7552,10 +7546,10 @@
     </row>
     <row r="264" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>13</v>
-      </c>
-      <c r="B264" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B264" s="6">
+        <v>45</v>
       </c>
       <c r="C264" s="1">
         <v>0</v>
@@ -7578,10 +7572,10 @@
     </row>
     <row r="265" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>13</v>
-      </c>
-      <c r="B265" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B265" s="6">
+        <v>45</v>
       </c>
       <c r="C265" s="1">
         <v>0</v>
@@ -7604,10 +7598,10 @@
     </row>
     <row r="266" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>13</v>
-      </c>
-      <c r="B266" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B266" s="6">
+        <v>45</v>
       </c>
       <c r="C266" s="1">
         <v>0</v>
@@ -7630,10 +7624,10 @@
     </row>
     <row r="267" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>13</v>
-      </c>
-      <c r="B267" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B267" s="6">
+        <v>45</v>
       </c>
       <c r="C267" s="1">
         <v>0</v>
@@ -7656,10 +7650,10 @@
     </row>
     <row r="268" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>13</v>
-      </c>
-      <c r="B268" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B268" s="6">
+        <v>45</v>
       </c>
       <c r="C268" s="1">
         <v>0</v>
@@ -7682,10 +7676,10 @@
     </row>
     <row r="269" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>13</v>
-      </c>
-      <c r="B269" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B269" s="6">
+        <v>45</v>
       </c>
       <c r="C269" s="1">
         <v>0</v>
@@ -7708,10 +7702,10 @@
     </row>
     <row r="270" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>13</v>
-      </c>
-      <c r="B270" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B270" s="6">
+        <v>45</v>
       </c>
       <c r="C270" s="1">
         <v>0</v>
@@ -7734,10 +7728,10 @@
     </row>
     <row r="271" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>13</v>
-      </c>
-      <c r="B271" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B271" s="6">
+        <v>45</v>
       </c>
       <c r="C271" s="1">
         <v>0</v>
@@ -7760,10 +7754,10 @@
     </row>
     <row r="272" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>13</v>
-      </c>
-      <c r="B272" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B272" s="6">
+        <v>45</v>
       </c>
       <c r="C272" s="1">
         <v>0</v>
@@ -7786,10 +7780,10 @@
     </row>
     <row r="273" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>13</v>
-      </c>
-      <c r="B273" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B273" s="6">
+        <v>45</v>
       </c>
       <c r="C273" s="1">
         <v>0</v>
@@ -7812,10 +7806,10 @@
     </row>
     <row r="274" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>13</v>
-      </c>
-      <c r="B274" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B274" s="6">
+        <v>45</v>
       </c>
       <c r="C274" s="1">
         <v>0</v>
@@ -7838,10 +7832,10 @@
     </row>
     <row r="275" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>13</v>
-      </c>
-      <c r="B275" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B275" s="6">
+        <v>45</v>
       </c>
       <c r="C275" s="1">
         <v>0</v>
@@ -7864,10 +7858,10 @@
     </row>
     <row r="276" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>13</v>
-      </c>
-      <c r="B276" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B276" s="6">
+        <v>45</v>
       </c>
       <c r="C276" s="1">
         <v>0</v>
@@ -7890,10 +7884,10 @@
     </row>
     <row r="277" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>13</v>
-      </c>
-      <c r="B277" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B277" s="6">
+        <v>45</v>
       </c>
       <c r="C277" s="1">
         <v>0</v>
@@ -7916,10 +7910,10 @@
     </row>
     <row r="278" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>13</v>
-      </c>
-      <c r="B278" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B278" s="6">
+        <v>45</v>
       </c>
       <c r="C278" s="1">
         <v>0</v>
@@ -7942,10 +7936,10 @@
     </row>
     <row r="279" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>13</v>
-      </c>
-      <c r="B279" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B279" s="6">
+        <v>45</v>
       </c>
       <c r="C279" s="1">
         <v>0</v>
@@ -7968,10 +7962,10 @@
     </row>
     <row r="280" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>13</v>
-      </c>
-      <c r="B280" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B280" s="6">
+        <v>45</v>
       </c>
       <c r="C280" s="1">
         <v>0</v>
@@ -7994,10 +7988,10 @@
     </row>
     <row r="281" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>13</v>
-      </c>
-      <c r="B281" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B281" s="6">
+        <v>45</v>
       </c>
       <c r="C281" s="1">
         <v>0</v>
@@ -8020,10 +8014,10 @@
     </row>
     <row r="282" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>13</v>
-      </c>
-      <c r="B282" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B282" s="6">
+        <v>45</v>
       </c>
       <c r="C282" s="1">
         <v>0</v>
@@ -8046,10 +8040,10 @@
     </row>
     <row r="283" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>13</v>
-      </c>
-      <c r="B283" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B283" s="6">
+        <v>45</v>
       </c>
       <c r="C283" s="1">
         <v>0</v>
@@ -8072,10 +8066,10 @@
     </row>
     <row r="284" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>13</v>
-      </c>
-      <c r="B284" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B284" s="6">
+        <v>45</v>
       </c>
       <c r="C284" s="1">
         <v>0</v>
@@ -8098,10 +8092,10 @@
     </row>
     <row r="285" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>13</v>
-      </c>
-      <c r="B285" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B285" s="6">
+        <v>45</v>
       </c>
       <c r="C285" s="1">
         <v>0</v>
@@ -8124,10 +8118,10 @@
     </row>
     <row r="286" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>13</v>
-      </c>
-      <c r="B286" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B286" s="6">
+        <v>45</v>
       </c>
       <c r="C286" s="1">
         <v>0</v>
@@ -8150,10 +8144,10 @@
     </row>
     <row r="287" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>13</v>
-      </c>
-      <c r="B287" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B287" s="6">
+        <v>45</v>
       </c>
       <c r="C287" s="1">
         <v>0</v>
@@ -8176,10 +8170,10 @@
     </row>
     <row r="288" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>13</v>
-      </c>
-      <c r="B288" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B288" s="6">
+        <v>45</v>
       </c>
       <c r="C288" s="1">
         <v>0</v>
@@ -8202,10 +8196,10 @@
     </row>
     <row r="289" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>13</v>
-      </c>
-      <c r="B289" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B289" s="6">
+        <v>45</v>
       </c>
       <c r="C289" s="1">
         <v>0</v>
@@ -8228,10 +8222,10 @@
     </row>
     <row r="290" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>13</v>
-      </c>
-      <c r="B290" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B290" s="6">
+        <v>45</v>
       </c>
       <c r="C290" s="1">
         <v>0</v>
@@ -8254,10 +8248,10 @@
     </row>
     <row r="291" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>13</v>
-      </c>
-      <c r="B291" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B291" s="6">
+        <v>45</v>
       </c>
       <c r="C291" s="1">
         <v>0</v>
@@ -8280,10 +8274,10 @@
     </row>
     <row r="292" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>13</v>
-      </c>
-      <c r="B292" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B292" s="6">
+        <v>45</v>
       </c>
       <c r="C292" s="1">
         <v>0</v>
@@ -8306,10 +8300,10 @@
     </row>
     <row r="293" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>13</v>
-      </c>
-      <c r="B293" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B293" s="6">
+        <v>45</v>
       </c>
       <c r="C293" s="1">
         <v>0</v>
@@ -8332,10 +8326,10 @@
     </row>
     <row r="294" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>13</v>
-      </c>
-      <c r="B294" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B294" s="6">
+        <v>45</v>
       </c>
       <c r="C294" s="1">
         <v>0</v>
@@ -8358,10 +8352,10 @@
     </row>
     <row r="295" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>13</v>
-      </c>
-      <c r="B295" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B295" s="6">
+        <v>45</v>
       </c>
       <c r="C295" s="1">
         <v>0</v>
@@ -8384,10 +8378,10 @@
     </row>
     <row r="296" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>13</v>
-      </c>
-      <c r="B296" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B296" s="6">
+        <v>45</v>
       </c>
       <c r="C296" s="1">
         <v>0</v>
@@ -8410,10 +8404,10 @@
     </row>
     <row r="297" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>13</v>
-      </c>
-      <c r="B297" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B297" s="6">
+        <v>45</v>
       </c>
       <c r="C297" s="1">
         <v>0</v>
@@ -8436,10 +8430,10 @@
     </row>
     <row r="298" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>13</v>
-      </c>
-      <c r="B298" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B298" s="6">
+        <v>45</v>
       </c>
       <c r="C298" s="1">
         <v>0</v>
@@ -8462,10 +8456,10 @@
     </row>
     <row r="299" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>13</v>
-      </c>
-      <c r="B299" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B299" s="6">
+        <v>45</v>
       </c>
       <c r="C299" s="1">
         <v>0</v>
@@ -8488,10 +8482,10 @@
     </row>
     <row r="300" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>13</v>
-      </c>
-      <c r="B300" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B300" s="6">
+        <v>45</v>
       </c>
       <c r="C300" s="1">
         <v>0</v>
@@ -8514,10 +8508,10 @@
     </row>
     <row r="301" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>13</v>
-      </c>
-      <c r="B301" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B301" s="6">
+        <v>45</v>
       </c>
       <c r="C301" s="1">
         <v>0</v>
@@ -8540,10 +8534,10 @@
     </row>
     <row r="302" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>13</v>
-      </c>
-      <c r="B302" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B302" s="6">
+        <v>45</v>
       </c>
       <c r="C302" s="1">
         <v>0</v>
@@ -8566,10 +8560,10 @@
     </row>
     <row r="303" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>13</v>
-      </c>
-      <c r="B303" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B303" s="6">
+        <v>45</v>
       </c>
       <c r="C303" s="1">
         <v>0</v>
@@ -8592,10 +8586,10 @@
     </row>
     <row r="304" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>13</v>
-      </c>
-      <c r="B304" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B304" s="6">
+        <v>45</v>
       </c>
       <c r="C304" s="1">
         <v>0</v>
@@ -8618,10 +8612,10 @@
     </row>
     <row r="305" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>13</v>
-      </c>
-      <c r="B305" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B305" s="6">
+        <v>45</v>
       </c>
       <c r="C305" s="1">
         <v>0</v>
@@ -8644,10 +8638,10 @@
     </row>
     <row r="306" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>13</v>
-      </c>
-      <c r="B306" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B306" s="6">
+        <v>45</v>
       </c>
       <c r="C306" s="1">
         <v>0</v>
@@ -8670,10 +8664,10 @@
     </row>
     <row r="307" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>13</v>
-      </c>
-      <c r="B307" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B307" s="6">
+        <v>45</v>
       </c>
       <c r="C307" s="1">
         <v>0</v>
@@ -8696,10 +8690,10 @@
     </row>
     <row r="308" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>13</v>
-      </c>
-      <c r="B308" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B308" s="6">
+        <v>45</v>
       </c>
       <c r="C308" s="1">
         <v>0</v>
@@ -8722,10 +8716,10 @@
     </row>
     <row r="309" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>13</v>
-      </c>
-      <c r="B309" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B309" s="6">
+        <v>45</v>
       </c>
       <c r="C309" s="1">
         <v>0</v>
@@ -8748,10 +8742,10 @@
     </row>
     <row r="310" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>13</v>
-      </c>
-      <c r="B310" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B310" s="6">
+        <v>45</v>
       </c>
       <c r="C310" s="1">
         <v>0</v>
@@ -8774,10 +8768,10 @@
     </row>
     <row r="311" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>13</v>
-      </c>
-      <c r="B311" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B311" s="6">
+        <v>45</v>
       </c>
       <c r="C311" s="1">
         <v>0</v>
@@ -8800,10 +8794,10 @@
     </row>
     <row r="312" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>13</v>
-      </c>
-      <c r="B312" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B312" s="6">
+        <v>45</v>
       </c>
       <c r="C312" s="1">
         <v>0</v>
@@ -8826,10 +8820,10 @@
     </row>
     <row r="313" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>13</v>
-      </c>
-      <c r="B313" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B313" s="6">
+        <v>45</v>
       </c>
       <c r="C313" s="1">
         <v>0</v>
@@ -8857,15 +8851,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -8915,7 +8900,32 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe">N4XJ6CXEYHH6-631025465-499113</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe">
+      <Url>https://artedrone.sharepoint.com/sites/SharepointArtedrone/_layouts/15/DocIdRedir.aspx?ID=N4XJ6CXEYHH6-631025465-499113</Url>
+      <Description>N4XJ6CXEYHH6-631025465-499113</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f867db0-d780-48fe-a112-754d1799c19e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005980ED226863A74FA2F9CA9139548579" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0242ed82f3266fd060e887ae3e26cb2b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="79361c6c-fea3-4edf-b4fa-5821e39e9bfe" xmlns:ns3="7f867db0-d780-48fe-a112-754d1799c19e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22c66529a84d53b789930f0e5aa4c2cf" ns2:_="" ns3:_="">
     <xsd:import namespace="79361c6c-fea3-4edf-b4fa-5821e39e9bfe"/>
@@ -9181,23 +9191,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe">N4XJ6CXEYHH6-631025465-499113</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe">
-      <Url>https://artedrone.sharepoint.com/sites/SharepointArtedrone/_layouts/15/DocIdRedir.aspx?ID=N4XJ6CXEYHH6-631025465-499113</Url>
-      <Description>N4XJ6CXEYHH6-631025465-499113</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="79361c6c-fea3-4edf-b4fa-5821e39e9bfe" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f867db0-d780-48fe-a112-754d1799c19e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7855C3A7-43F2-4E39-B3EE-8D5AE289D659}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8128331-F855-46C9-83E5-1081B8762C26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9205,19 +9207,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7855C3A7-43F2-4E39-B3EE-8D5AE289D659}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A9C59E8-6087-4EFD-8CD7-56181A25F8B1}"/>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F56340EC-2E80-4BEE-AA2C-1B622E4607C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9226,4 +9216,23 @@
     <ds:schemaRef ds:uri="7f867db0-d780-48fe-a112-754d1799c19e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A9C59E8-6087-4EFD-8CD7-56181A25F8B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="79361c6c-fea3-4edf-b4fa-5821e39e9bfe"/>
+    <ds:schemaRef ds:uri="7f867db0-d780-48fe-a112-754d1799c19e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>